<commit_message>
Model Test with larger init CSVs
</commit_message>
<xml_diff>
--- a/InstantiateAgents.xlsx
+++ b/InstantiateAgents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziyan\PycharmProjects\AAE560-Proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CC09C84-5A42-4156-A782-7B783DF6DE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E00D62-ADB8-4E3B-B412-1FBED7889FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FixNodes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -69,6 +69,24 @@
   </si>
   <si>
     <t>SpaceY</t>
+  </si>
+  <si>
+    <t>TestTrans2</t>
+  </si>
+  <si>
+    <t>VarTest2</t>
+  </si>
+  <si>
+    <t>FixTest2</t>
+  </si>
+  <si>
+    <t>RedOrigin</t>
+  </si>
+  <si>
+    <t>TestTrans3</t>
+  </si>
+  <si>
+    <t>ChadGalactic</t>
   </si>
 </sst>
 </file>
@@ -386,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,6 +446,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3">
+        <v>25000</v>
+      </c>
+      <c r="D3">
+        <v>4000</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -435,10 +470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F404E483-C86C-48D7-9757-3C299C10ECFE}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,6 +512,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>800</v>
+      </c>
+      <c r="C3">
+        <v>950</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -484,15 +536,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05EFA847-20D2-4CF7-B2E4-F3CBAE1D7EAD}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -541,6 +594,52 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+      <c r="C3">
+        <v>350</v>
+      </c>
+      <c r="D3">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Step function and model step function written. They are "working" the agents move but sometimes hangups due to trig domain errors in Phys.py. Plese fix
</commit_message>
<xml_diff>
--- a/InstantiateAgents.xlsx
+++ b/InstantiateAgents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziyan\PycharmProjects\AAE560-Proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E00D62-ADB8-4E3B-B412-1FBED7889FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2BE291-4744-4D1D-9EAF-26CDCDADC387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,28 @@
     <sheet name="VarNodes" sheetId="3" r:id="rId2"/>
     <sheet name="Transporters" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -63,9 +74,6 @@
   </si>
   <si>
     <t>TestTrans1</t>
-  </si>
-  <si>
-    <t>earth</t>
   </si>
   <si>
     <t>SpaceY</t>
@@ -407,7 +415,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,10 +442,12 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <f>6378.14+300</f>
+        <v>6678.14</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <f>300+6378.14</f>
+        <v>6678.14</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -448,7 +458,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>10000</v>
@@ -473,7 +483,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,10 +510,12 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <f>200+6378.14</f>
+        <v>6578.14</v>
       </c>
       <c r="C2">
-        <v>350</v>
+        <f>350+6378.14</f>
+        <v>6728.14</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -514,13 +526,15 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>800</v>
+        <f>800+6378.14</f>
+        <v>7178.14</v>
       </c>
       <c r="C3">
-        <v>950</v>
+        <f>950+6378.14</f>
+        <v>7328.14</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -539,7 +553,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,65 +593,71 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>-250</v>
+        <f>-(250+6378.14)</f>
+        <v>-6628.14</v>
       </c>
       <c r="D2">
-        <v>250</v>
+        <f>250+6378.14</f>
+        <v>6628.14</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>350</v>
+        <f>350+6378.14</f>
+        <v>6728.14</v>
       </c>
       <c r="D3">
-        <v>120</v>
+        <f>120+6378.14</f>
+        <v>6498.14</v>
       </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>300</v>
+        <f>300+6378.14</f>
+        <v>6678.14</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <f>200+6378.14</f>
+        <v>6578.14</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>